<commit_message>
Calibrate Armenia for total population size
</commit_message>
<xml_diff>
--- a/autumn/xls/data_armenia.xlsx
+++ b/autumn/xls/data_armenia.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rragonnet\Google Drive\GitHub\AuTuMN\autumn\xls\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="795" windowWidth="20370" windowHeight="7050" tabRatio="807"/>
+    <workbookView xWindow="120" yWindow="792" windowWidth="20376" windowHeight="7056" tabRatio="807"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="4" r:id="rId1"/>
     <sheet name="time_variants" sheetId="2" r:id="rId2"/>
     <sheet name="dropdown_lists" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>yes</t>
   </si>
@@ -67,6 +72,36 @@
   </si>
   <si>
     <t>upper</t>
+  </si>
+  <si>
+    <t>start_mdr_introduce_time</t>
+  </si>
+  <si>
+    <t>Calendar year that MDR-TB first begins to emerge</t>
+  </si>
+  <si>
+    <t>end_mdr_introduce_time</t>
+  </si>
+  <si>
+    <t>Calendar year that MDR-TB amplification reaches full parameter value</t>
+  </si>
+  <si>
+    <t>program_prop_death_reporting</t>
+  </si>
+  <si>
+    <t>Proportion of TB-related deaths not already under treatment that are correctly reported as such</t>
+  </si>
+  <si>
+    <t>susceptible_fully</t>
+  </si>
+  <si>
+    <t>Starting population of fully susceptible persons (essentially the starting population size)</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
+    <t>Seed of patients with active TB</t>
   </si>
 </sst>
 </file>
@@ -76,7 +111,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,8 +182,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="3" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -172,8 +214,26 @@
         <fgColor rgb="FFFFCC99"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -264,6 +324,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="664">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -931,7 +1000,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
@@ -948,6 +1017,24 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="5" borderId="0" xfId="663" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="6" borderId="0" xfId="663" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="9" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="5" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="5" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="5" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="5" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="664">
     <cellStyle name="Comma 2" xfId="4"/>
@@ -1621,6 +1708,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1668,7 +1758,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1703,7 +1793,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1912,20 +2002,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="51.28515625" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="93.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="93.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>6</v>
       </c>
@@ -1942,12 +2032,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="8">
-        <v>6.6</v>
+        <v>6.4</v>
       </c>
       <c r="C2" s="8">
         <v>5</v>
@@ -1959,7 +2049,82 @@
         <v>9</v>
       </c>
     </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="17">
+        <v>0.6</v>
+      </c>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="13">
+        <v>1950</v>
+      </c>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="13">
+        <v>1955</v>
+      </c>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="19">
+        <v>1300000</v>
+      </c>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="22">
+        <v>3</v>
+      </c>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="21" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:D5">
+      <formula1>-10000</formula1>
+      <formula2>10000</formula2>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:D7">
+      <formula1>0</formula1>
+      <formula2>10000000000</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1979,31 +2144,31 @@
       <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="56" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" style="2" customWidth="1"/>
-    <col min="4" max="5" width="7.42578125" style="1" customWidth="1"/>
+    <col min="4" max="5" width="7.44140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="1" customWidth="1"/>
-    <col min="8" max="9" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.42578125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.7109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="7.28515625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="7.42578125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.140625" style="1" customWidth="1"/>
-    <col min="19" max="20" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="7.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.44140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="7.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.6640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="7.33203125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="7.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="7.44140625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="7.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.109375" style="1" customWidth="1"/>
+    <col min="19" max="20" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="8" style="1" customWidth="1"/>
-    <col min="24" max="24" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7.85546875" style="1" customWidth="1"/>
-    <col min="28" max="16384" width="9.140625" style="1"/>
+    <col min="24" max="24" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.88671875" style="1" customWidth="1"/>
+    <col min="28" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -2113,7 +2278,7 @@
       <selection activeCell="D4" sqref="A2:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">

</xml_diff>

<commit_message>
Fix death on treatment MDR default data
Death rate too high for MDR deaths on treatment.
</commit_message>
<xml_diff>
--- a/autumn/xls/data_armenia.xlsx
+++ b/autumn/xls/data_armenia.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="795" windowWidth="20370" windowHeight="7050" tabRatio="807"/>
+    <workbookView xWindow="120" yWindow="795" windowWidth="20370" windowHeight="7050" tabRatio="807" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="4" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>yes</t>
   </si>
@@ -100,9 +100,6 @@
   </si>
   <si>
     <t>tb_prop_amplification</t>
-  </si>
-  <si>
-    <t>program_perc_treatment_death_mdr</t>
   </si>
   <si>
     <t>program_perc_detect</t>
@@ -2018,8 +2015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2156,7 +2153,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" s="18">
         <v>5</v>
@@ -2218,13 +2215,13 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:AB4"/>
+  <dimension ref="A1:AB3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4:XFD4"/>
+      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2344,44 +2341,30 @@
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="M2" s="1">
+      <c r="Z2" s="1">
+        <v>80</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="23"/>
+      <c r="D3" s="24"/>
+      <c r="X3" s="25">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="26">
         <v>20</v>
       </c>
-      <c r="P2" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z3" s="1">
-        <v>80</v>
-      </c>
-      <c r="AA3" s="1">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="4" spans="1:28" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="24"/>
-      <c r="X4" s="25">
-        <v>0</v>
-      </c>
-      <c r="Z4" s="26">
-        <v>20</v>
-      </c>
-      <c r="AA4" s="26"/>
-      <c r="AB4" s="26"/>
+      <c r="AA3" s="26"/>
+      <c r="AB3" s="26"/>
     </row>
   </sheetData>
   <dataValidations xWindow="382" yWindow="552" count="2">

</xml_diff>

<commit_message>
Add stratification for treatment history
No functionality yet or literature review. However, entire model can now be stratified by treatment history.
</commit_message>
<xml_diff>
--- a/autumn/xls/data_armenia.xlsx
+++ b/autumn/xls/data_armenia.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="795" windowWidth="20370" windowHeight="7050" tabRatio="807" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="795" windowWidth="20370" windowHeight="7050" tabRatio="807"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="4" r:id="rId1"/>
@@ -1997,8 +1997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2199,7 +2199,7 @@
   </sheetPr>
   <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>

<commit_message>
Remove all old terms for MDR introduction
Remove all the MDR introduction end times and change the introduction time to just mdr_introduce_time.
</commit_message>
<xml_diff>
--- a/autumn/xls/data_armenia.xlsx
+++ b/autumn/xls/data_armenia.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>yes</t>
   </si>
@@ -69,18 +69,9 @@
     <t>upper</t>
   </si>
   <si>
-    <t>start_mdr_introduce_time</t>
-  </si>
-  <si>
     <t>Calendar year that MDR-TB first begins to emerge</t>
   </si>
   <si>
-    <t>end_mdr_introduce_time</t>
-  </si>
-  <si>
-    <t>Calendar year that MDR-TB amplification reaches full parameter value</t>
-  </si>
-  <si>
     <t>program_prop_death_reporting</t>
   </si>
   <si>
@@ -106,6 +97,9 @@
   </si>
   <si>
     <t>age_breakpoints</t>
+  </si>
+  <si>
+    <t>mdr_introduce_time</t>
   </si>
 </sst>
 </file>
@@ -1995,10 +1989,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2044,7 +2038,7 @@
     </row>
     <row r="3" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B3" s="17">
         <v>0.6</v>
@@ -2052,12 +2046,12 @@
       <c r="C3" s="17"/>
       <c r="D3" s="17"/>
       <c r="E3" s="9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B4" s="8">
         <v>0.55000000000000004</v>
@@ -2071,7 +2065,7 @@
     </row>
     <row r="5" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B5" s="13">
         <v>1900</v>
@@ -2079,23 +2073,23 @@
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
       <c r="E5" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F5" s="20"/>
       <c r="G5" s="20"/>
       <c r="H5" s="20"/>
     </row>
     <row r="6" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A6" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="13">
-        <v>1905</v>
-      </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="15" t="s">
+      <c r="A6" s="18" t="s">
         <v>20</v>
+      </c>
+      <c r="B6" s="19">
+        <v>1300000</v>
+      </c>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="18" t="s">
+        <v>21</v>
       </c>
       <c r="F6" s="20"/>
       <c r="G6" s="20"/>
@@ -2103,48 +2097,42 @@
     </row>
     <row r="7" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="19">
-        <v>1300000</v>
+        <v>3</v>
       </c>
       <c r="C7" s="21"/>
       <c r="D7" s="21"/>
       <c r="E7" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F7" s="20"/>
       <c r="G7" s="20"/>
       <c r="H7" s="20"/>
     </row>
-    <row r="8" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="19">
-        <v>3</v>
-      </c>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
+      <c r="B8" s="18">
+        <v>5</v>
+      </c>
+      <c r="C8" s="18">
+        <v>15</v>
+      </c>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="18">
-        <v>5</v>
-      </c>
-      <c r="C9" s="18">
-        <v>15</v>
-      </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
+      <c r="A9" s="20"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="20"/>
@@ -2166,23 +2154,13 @@
       <c r="G11" s="20"/>
       <c r="H11" s="20"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="20"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:D6">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:D5">
       <formula1>-10000</formula1>
       <formula2>10000</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:D8">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:D7">
       <formula1>0</formula1>
       <formula2>10000000000</formula2>
     </dataValidation>
@@ -2318,7 +2296,7 @@
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>

</xml_diff>